<commit_message>
Add visualisation, stacked frames, recalibrate file reading and self storage
</commit_message>
<xml_diff>
--- a/End-Use technologies DataBase.xlsx
+++ b/End-Use technologies DataBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertrehnberg/Desktop/projekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AB9FE6-EA37-1548-AD68-8197A32F729F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837DDE48-B9E6-2D49-A116-2F8879BC4D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SpaceHeating" sheetId="1" r:id="rId1"/>
@@ -1632,14 +1632,14 @@
     <xf numFmtId="0" fontId="73" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="75" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="76" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1860,7 +1860,7 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2042,7 +2042,7 @@
     <col min="7" max="7" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -2362,7 +2362,7 @@
       <c r="A2" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="98" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -2385,7 +2385,7 @@
       <c r="A3" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="99" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -2408,7 +2408,7 @@
       <c r="A4" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="98" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -2431,7 +2431,7 @@
       <c r="A5" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="100" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -2468,8 +2468,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -2487,7 +2487,7 @@
         <v>291</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -3550,7 +3550,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C16"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -4014,7 +4014,7 @@
     <col min="10" max="10" width="116.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" ht="15">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" ht="13">
       <c r="A3" s="15" t="s">
         <v>141</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" ht="13">
       <c r="A9" s="34" t="s">
         <v>154</v>
       </c>
@@ -4322,7 +4322,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" ht="16">
       <c r="A12" s="63" t="s">
         <v>160</v>
       </c>
@@ -4459,7 +4459,7 @@
     <col min="7" max="7" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="15">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="16">
       <c r="A11" s="74"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1">
@@ -4649,7 +4649,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="16">
       <c r="A14" s="75" t="s">
         <v>191</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="13">
       <c r="A3" s="81" t="s">
         <v>204</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="13">
       <c r="A4" s="81" t="s">
         <v>206</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="13">
       <c r="A6" s="34" t="s">
         <v>210</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="16">
       <c r="A7" s="83" t="s">
         <v>211</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="13">
       <c r="A9" s="34" t="s">
         <v>215</v>
       </c>
@@ -5031,17 +5031,17 @@
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1">
       <c r="A18" s="88"/>
-      <c r="B18" s="98" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="98">
+      <c r="B18" s="101" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="101">
         <v>18</v>
       </c>
-      <c r="D18" s="100">
+      <c r="D18" s="103">
         <f>(((118*120/(6343*18))*100))</f>
         <v>12.402123075306113</v>
       </c>
-      <c r="E18" s="100">
+      <c r="E18" s="103">
         <f>1769000/17000</f>
         <v>104.05882352941177</v>
       </c>
@@ -5053,10 +5053,10 @@
       <c r="A19" s="88" t="s">
         <v>237</v>
       </c>
-      <c r="B19" s="99"/>
-      <c r="C19" s="99"/>
-      <c r="D19" s="99"/>
-      <c r="E19" s="99"/>
+      <c r="B19" s="102"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="102"/>
+      <c r="E19" s="102"/>
       <c r="F19" s="3" t="s">
         <v>238</v>
       </c>
@@ -5065,10 +5065,10 @@
       <c r="A20" s="88" t="s">
         <v>239</v>
       </c>
-      <c r="B20" s="99"/>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="99"/>
+      <c r="B20" s="102"/>
+      <c r="C20" s="102"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="102"/>
       <c r="F20" s="8" t="s">
         <v>240</v>
       </c>
@@ -5077,17 +5077,17 @@
       <c r="A21" s="88" t="s">
         <v>241</v>
       </c>
-      <c r="B21" s="98" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="98">
+      <c r="B21" s="101" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="101">
         <v>25</v>
       </c>
-      <c r="D21" s="100">
+      <c r="D21" s="103">
         <f>(((124*125/(6343*25))*100))</f>
         <v>9.7745546271480368</v>
       </c>
-      <c r="E21" s="99"/>
+      <c r="E21" s="102"/>
       <c r="F21" s="3" t="s">
         <v>242</v>
       </c>
@@ -5096,10 +5096,10 @@
       <c r="A22" s="88" t="s">
         <v>243</v>
       </c>
-      <c r="B22" s="99"/>
-      <c r="C22" s="99"/>
-      <c r="D22" s="99"/>
-      <c r="E22" s="99"/>
+      <c r="B22" s="102"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="102"/>
+      <c r="E22" s="102"/>
       <c r="F22" s="3" t="s">
         <v>238</v>
       </c>
@@ -5108,10 +5108,10 @@
       <c r="A23" s="88" t="s">
         <v>239</v>
       </c>
-      <c r="B23" s="99"/>
-      <c r="C23" s="99"/>
-      <c r="D23" s="99"/>
-      <c r="E23" s="99"/>
+      <c r="B23" s="102"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="102"/>
+      <c r="E23" s="102"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24" s="10" t="s">

</xml_diff>